<commit_message>
failed TestCase Class Add
</commit_message>
<xml_diff>
--- a/RedBus/Testdata/Data.xlsx
+++ b/RedBus/Testdata/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="8460" windowHeight="3030" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:H8"/>
 </workbook>
 </file>
 
@@ -355,7 +356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -392,7 +393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>